<commit_message>
entry 6 compound equivalents updated along with new prediction results
</commit_message>
<xml_diff>
--- a/Code_And_Data/Dataset/TestingData_WithPredictedResults.xlsx
+++ b/Code_And_Data/Dataset/TestingData_WithPredictedResults.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailmissouri-my.sharepoint.com/personal/ur48t_umsystem_edu/Documents/RA docs/Fall24_ResearchWork/Projects/AI_Chemistry/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/upasanaroy/Documents/AI_Chem_Github/Yield-Prediction/Code_And_Data/Dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{8F361212-6D1B-BC41-8A9E-911CF384579B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2BBA0BD7-4CCE-3D43-B0BB-ABB318270089}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02FC2780-6A02-974C-ABE2-EBAF0A242059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -197,9 +197,6 @@
     <t>Toluene</t>
   </si>
   <si>
-    <t>Benzenamine hydrochloride (1:1)</t>
-  </si>
-  <si>
     <t>Tetrahydrofuran:Water</t>
   </si>
   <si>
@@ -335,6 +332,9 @@
   </si>
   <si>
     <t>Predicted Reaction_Yield</t>
+  </si>
+  <si>
+    <t>Benzenamine hydrochloride</t>
   </si>
 </sst>
 </file>
@@ -704,10 +704,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1029,8 +1025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0284D173-9243-8145-8C4D-CC2D2BC9D4B7}">
   <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1057,13 +1053,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>84</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>85</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>2</v>
@@ -1090,10 +1086,10 @@
         <v>9</v>
       </c>
       <c r="M1" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="N1" s="46" t="s">
         <v>86</v>
-      </c>
-      <c r="N1" s="46" t="s">
-        <v>87</v>
       </c>
       <c r="O1" s="10" t="s">
         <v>10</v>
@@ -1292,28 +1288,28 @@
         <v>38</v>
       </c>
       <c r="B6" s="11">
-        <v>1</v>
+        <v>1.6</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>53</v>
+        <v>87</v>
       </c>
       <c r="D6" s="20">
         <v>1</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F6" s="21">
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
       <c r="G6" s="17" t="s">
         <v>49</v>
       </c>
       <c r="H6" s="11">
-        <v>2</v>
+        <v>3.3</v>
       </c>
       <c r="I6" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J6" s="21">
         <v>0.01</v>
@@ -1328,10 +1324,10 @@
         <v>100</v>
       </c>
       <c r="N6" s="18">
-        <v>89.904756000000006</v>
+        <v>72.972087999999999</v>
       </c>
       <c r="O6" s="23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="20">
@@ -1342,13 +1338,13 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D7" s="20">
         <v>1</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F7" s="21">
         <v>1</v>
@@ -1360,7 +1356,7 @@
         <v>0</v>
       </c>
       <c r="I7" s="21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J7" s="21">
         <v>0.625</v>
@@ -1378,30 +1374,30 @@
         <v>66.903041999999999</v>
       </c>
       <c r="O7" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="22">
       <c r="A8" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="27">
+        <v>1</v>
+      </c>
+      <c r="C8" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="B8" s="27">
-        <v>1</v>
-      </c>
-      <c r="C8" s="28" t="s">
+      <c r="D8" s="29">
+        <v>1</v>
+      </c>
+      <c r="E8" s="30" t="s">
         <v>65</v>
-      </c>
-      <c r="D8" s="29">
-        <v>1</v>
-      </c>
-      <c r="E8" s="30" t="s">
-        <v>66</v>
       </c>
       <c r="F8" s="31">
         <v>1.23</v>
       </c>
       <c r="G8" s="30" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H8" s="31">
         <v>2.52</v>
@@ -1425,30 +1421,30 @@
         <v>83.967907999999994</v>
       </c>
       <c r="O8" s="33" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="22">
       <c r="A9" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B9" s="27">
         <v>1</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D9" s="29">
         <v>1</v>
       </c>
       <c r="E9" s="30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F9" s="31">
         <v>1.23</v>
       </c>
       <c r="G9" s="30" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H9" s="31">
         <v>2.52</v>
@@ -1472,7 +1468,7 @@
         <v>90.326130000000006</v>
       </c>
       <c r="O9" s="33" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="22">
@@ -1483,19 +1479,19 @@
         <v>1</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D10" s="29">
         <v>1</v>
       </c>
       <c r="E10" s="30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F10" s="31">
         <v>1.23</v>
       </c>
       <c r="G10" s="30" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H10" s="31">
         <v>2.52</v>
@@ -1519,30 +1515,30 @@
         <v>81.986705000000001</v>
       </c>
       <c r="O10" s="33" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="22">
       <c r="A11" s="26" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B11" s="27">
         <v>1</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D11" s="29">
         <v>1</v>
       </c>
       <c r="E11" s="30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F11" s="31">
         <v>1.23</v>
       </c>
       <c r="G11" s="30" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H11" s="31">
         <v>2.52</v>
@@ -1566,36 +1562,36 @@
         <v>63.183840000000004</v>
       </c>
       <c r="O11" s="33" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="20">
       <c r="A12" s="26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B12" s="27">
         <v>1.1000000000000001</v>
       </c>
       <c r="C12" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="29">
+        <v>1</v>
+      </c>
+      <c r="E12" s="30" t="s">
         <v>72</v>
-      </c>
-      <c r="D12" s="29">
-        <v>1</v>
-      </c>
-      <c r="E12" s="30" t="s">
-        <v>73</v>
       </c>
       <c r="F12" s="31">
         <v>1.1000000000000001</v>
       </c>
       <c r="G12" s="30" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H12" s="31">
         <v>3.1</v>
       </c>
       <c r="I12" s="31" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J12" s="31">
         <v>0.5</v>
@@ -1613,7 +1609,7 @@
         <v>96.954841000000002</v>
       </c>
       <c r="O12" s="26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="20">
@@ -1865,7 +1861,7 @@
         <v>2</v>
       </c>
       <c r="E18" s="41" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F18" s="35">
         <v>1.25</v>
@@ -1942,18 +1938,18 @@
         <v>54.428367999999999</v>
       </c>
       <c r="O19" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="22">
       <c r="A20" s="39" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B20" s="42">
         <v>1</v>
       </c>
       <c r="C20" s="43" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D20" s="35">
         <v>1</v>
@@ -1965,13 +1961,13 @@
         <v>1.3</v>
       </c>
       <c r="G20" s="39" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H20" s="42">
         <v>2</v>
       </c>
       <c r="I20" s="31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J20" s="42">
         <v>0.5</v>
@@ -1989,7 +1985,7 @@
         <v>71.149499000000006</v>
       </c>
       <c r="O20" s="45" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="22">
@@ -2000,7 +1996,7 @@
         <v>1</v>
       </c>
       <c r="C21" s="39" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D21" s="35">
         <v>1</v>
@@ -2012,13 +2008,13 @@
         <v>1.3</v>
       </c>
       <c r="G21" s="39" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H21" s="42">
         <v>2</v>
       </c>
       <c r="I21" s="31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J21" s="42">
         <v>0.5</v>
@@ -2036,7 +2032,7 @@
         <v>87.434918999999994</v>
       </c>
       <c r="O21" s="45" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="20">
@@ -2059,6 +2055,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f006263b-6855-4f81-be49-4241caee7f23">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="dabe3c20-206e-48c2-bf8d-a29783c980eb" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DBC1E36CE2333A4DBCA9CD5063464EF8" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d9620bf27d4ff32933b9f2337e2be106">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f006263b-6855-4f81-be49-4241caee7f23" xmlns:ns3="dabe3c20-206e-48c2-bf8d-a29783c980eb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d08129629143736746fb52b30a130668" ns2:_="" ns3:_="">
     <xsd:import namespace="f006263b-6855-4f81-be49-4241caee7f23"/>
@@ -2281,27 +2297,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C683F71-BAD6-45A7-9C46-62C2D2F63BFF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="dabe3c20-206e-48c2-bf8d-a29783c980eb"/>
+    <ds:schemaRef ds:uri="f006263b-6855-4f81-be49-4241caee7f23"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f006263b-6855-4f81-be49-4241caee7f23">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="dabe3c20-206e-48c2-bf8d-a29783c980eb" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{65EBFEDB-1F62-4F1C-B496-B4021A8B8AE1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB92CAC3-9F74-4995-820F-13C750327611}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2318,29 +2339,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{65EBFEDB-1F62-4F1C-B496-B4021A8B8AE1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C683F71-BAD6-45A7-9C46-62C2D2F63BFF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="dabe3c20-206e-48c2-bf8d-a29783c980eb"/>
-    <ds:schemaRef ds:uri="f006263b-6855-4f81-be49-4241caee7f23"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>